<commit_message>
The corpus with dates first, for use in Voyant
</commit_message>
<xml_diff>
--- a/data/legal_instrument_index.xlsx
+++ b/data/legal_instrument_index.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benjaminmartin/Documents/Academic Work (non-diss)/Intl Ideas at UNESCO (VR 2020-2023)/INIDUN/unesco_data_collection/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0DC2D4E-6149-5D4E-9C80-3264736D310F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13B150D7-AF0F-2A4E-9999-9647F681621E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="16540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5720" yWindow="880" windowWidth="27640" windowHeight="16540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="legal_instrument_index" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="278">
   <si>
     <t>section_id</t>
   </si>
@@ -857,9 +857,6 @@
   </si>
   <si>
     <t>yes</t>
-  </si>
-  <si>
-    <t>no</t>
   </si>
 </sst>
 </file>
@@ -1702,10 +1699,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:J83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A65" sqref="A65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1846,31 +1844,31 @@
         <v>201</v>
       </c>
       <c r="B5">
-        <v>12949</v>
+        <v>15381</v>
       </c>
       <c r="C5" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
       <c r="D5" t="s">
         <v>15</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>277</v>
       </c>
       <c r="G5">
-        <v>1960</v>
+        <v>1952</v>
       </c>
       <c r="H5" s="1">
-        <v>22264</v>
+        <v>19243</v>
       </c>
       <c r="I5" t="s">
-        <v>17</v>
+        <v>91</v>
       </c>
       <c r="J5" t="s">
-        <v>105</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -1878,31 +1876,31 @@
         <v>201</v>
       </c>
       <c r="B6">
-        <v>13036</v>
+        <v>13637</v>
       </c>
       <c r="C6" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="D6" t="s">
         <v>15</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>277</v>
       </c>
       <c r="G6">
-        <v>1958</v>
+        <v>1954</v>
       </c>
       <c r="H6" s="1">
-        <v>21522</v>
+        <v>19858</v>
       </c>
       <c r="I6" t="s">
-        <v>17</v>
+        <v>114</v>
       </c>
       <c r="J6" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
@@ -1910,31 +1908,28 @@
         <v>201</v>
       </c>
       <c r="B7">
-        <v>13039</v>
+        <v>13062</v>
       </c>
       <c r="C7" t="s">
-        <v>93</v>
+        <v>230</v>
       </c>
       <c r="D7" t="s">
-        <v>15</v>
+        <v>128</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>94</v>
+        <v>231</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>277</v>
       </c>
       <c r="G7">
-        <v>1970</v>
+        <v>1956</v>
       </c>
       <c r="H7" s="1">
-        <v>25886</v>
-      </c>
-      <c r="I7" t="s">
-        <v>17</v>
+        <v>20794</v>
       </c>
       <c r="J7" t="s">
-        <v>95</v>
+        <v>232</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
@@ -1942,31 +1937,31 @@
         <v>201</v>
       </c>
       <c r="B8">
-        <v>13055</v>
+        <v>13036</v>
       </c>
       <c r="C8" t="s">
-        <v>79</v>
+        <v>109</v>
       </c>
       <c r="D8" t="s">
         <v>15</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>80</v>
+        <v>110</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>277</v>
       </c>
       <c r="G8">
-        <v>1972</v>
+        <v>1958</v>
       </c>
       <c r="H8" s="1">
-        <v>26619</v>
+        <v>21522</v>
       </c>
       <c r="I8" t="s">
         <v>17</v>
       </c>
       <c r="J8" t="s">
-        <v>81</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
@@ -1974,31 +1969,31 @@
         <v>201</v>
       </c>
       <c r="B9">
-        <v>13059</v>
+        <v>15395</v>
       </c>
       <c r="C9" t="s">
-        <v>47</v>
+        <v>106</v>
       </c>
       <c r="D9" t="s">
         <v>15</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>48</v>
+        <v>107</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>277</v>
       </c>
       <c r="G9">
-        <v>1989</v>
+        <v>1958</v>
       </c>
       <c r="H9" s="1">
-        <v>32822</v>
+        <v>21522</v>
       </c>
       <c r="I9" t="s">
         <v>17</v>
       </c>
       <c r="J9" t="s">
-        <v>49</v>
+        <v>108</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
@@ -2006,31 +2001,31 @@
         <v>201</v>
       </c>
       <c r="B10">
-        <v>13512</v>
+        <v>12949</v>
       </c>
       <c r="C10" t="s">
-        <v>76</v>
+        <v>103</v>
       </c>
       <c r="D10" t="s">
         <v>15</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>77</v>
+        <v>104</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>277</v>
       </c>
       <c r="G10">
-        <v>1974</v>
+        <v>1960</v>
       </c>
       <c r="H10" s="1">
-        <v>27229</v>
+        <v>22264</v>
       </c>
       <c r="I10" t="s">
-        <v>78</v>
+        <v>17</v>
       </c>
       <c r="J10" t="s">
-        <v>22</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
@@ -2038,31 +2033,28 @@
         <v>201</v>
       </c>
       <c r="B11">
-        <v>13514</v>
+        <v>13063</v>
       </c>
       <c r="C11" t="s">
-        <v>68</v>
+        <v>224</v>
       </c>
       <c r="D11" t="s">
-        <v>15</v>
+        <v>128</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>69</v>
+        <v>225</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>277</v>
       </c>
       <c r="G11">
-        <v>1976</v>
+        <v>1960</v>
       </c>
       <c r="H11" s="1">
-        <v>28111</v>
-      </c>
-      <c r="I11" t="s">
-        <v>70</v>
+        <v>22264</v>
       </c>
       <c r="J11" t="s">
-        <v>71</v>
+        <v>226</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
@@ -2070,31 +2062,28 @@
         <v>201</v>
       </c>
       <c r="B12">
-        <v>13516</v>
+        <v>13065</v>
       </c>
       <c r="C12" t="s">
-        <v>58</v>
+        <v>227</v>
       </c>
       <c r="D12" t="s">
-        <v>15</v>
+        <v>128</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>59</v>
+        <v>228</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>277</v>
       </c>
       <c r="G12">
-        <v>1979</v>
+        <v>1960</v>
       </c>
       <c r="H12" s="1">
-        <v>29210</v>
-      </c>
-      <c r="I12" t="s">
-        <v>17</v>
+        <v>22264</v>
       </c>
       <c r="J12" t="s">
-        <v>60</v>
+        <v>229</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
@@ -2102,31 +2091,31 @@
         <v>201</v>
       </c>
       <c r="B13">
-        <v>13517</v>
+        <v>13645</v>
       </c>
       <c r="C13" t="s">
-        <v>65</v>
+        <v>99</v>
       </c>
       <c r="D13" t="s">
         <v>15</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>66</v>
+        <v>100</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>277</v>
       </c>
       <c r="G13">
-        <v>1978</v>
+        <v>1961</v>
       </c>
       <c r="H13" s="1">
-        <v>28846</v>
+        <v>22580</v>
       </c>
       <c r="I13" t="s">
-        <v>17</v>
+        <v>101</v>
       </c>
       <c r="J13" t="s">
-        <v>67</v>
+        <v>102</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
@@ -2134,31 +2123,31 @@
         <v>201</v>
       </c>
       <c r="B14">
-        <v>13518</v>
+        <v>15321</v>
       </c>
       <c r="C14" t="s">
-        <v>54</v>
+        <v>96</v>
       </c>
       <c r="D14" t="s">
         <v>15</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>55</v>
+        <v>97</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>277</v>
       </c>
       <c r="G14">
-        <v>1981</v>
+        <v>1962</v>
       </c>
       <c r="H14" s="1">
-        <v>29925</v>
+        <v>22990</v>
       </c>
       <c r="I14" t="s">
-        <v>56</v>
+        <v>17</v>
       </c>
       <c r="J14" t="s">
-        <v>57</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
@@ -2166,31 +2155,28 @@
         <v>201</v>
       </c>
       <c r="B15">
-        <v>13520</v>
+        <v>13067</v>
       </c>
       <c r="C15" t="s">
-        <v>40</v>
+        <v>221</v>
       </c>
       <c r="D15" t="s">
-        <v>15</v>
+        <v>128</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>41</v>
+        <v>222</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>277</v>
       </c>
       <c r="G15">
-        <v>2001</v>
+        <v>1962</v>
       </c>
       <c r="H15" s="1">
-        <v>37197</v>
-      </c>
-      <c r="I15" t="s">
-        <v>17</v>
+        <v>22991</v>
       </c>
       <c r="J15" t="s">
-        <v>42</v>
+        <v>223</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
@@ -2198,31 +2184,28 @@
         <v>201</v>
       </c>
       <c r="B16">
-        <v>13522</v>
+        <v>13068</v>
       </c>
       <c r="C16" t="s">
-        <v>43</v>
+        <v>215</v>
       </c>
       <c r="D16" t="s">
-        <v>15</v>
+        <v>128</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>44</v>
+        <v>216</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>277</v>
       </c>
       <c r="G16">
-        <v>1997</v>
+        <v>1964</v>
       </c>
       <c r="H16" s="1">
-        <v>35531</v>
-      </c>
-      <c r="I16" t="s">
-        <v>45</v>
+        <v>23700</v>
       </c>
       <c r="J16" t="s">
-        <v>46</v>
+        <v>217</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
@@ -2230,31 +2213,28 @@
         <v>201</v>
       </c>
       <c r="B17">
-        <v>13523</v>
+        <v>13083</v>
       </c>
       <c r="C17" t="s">
-        <v>50</v>
+        <v>218</v>
       </c>
       <c r="D17" t="s">
-        <v>15</v>
+        <v>128</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>51</v>
+        <v>219</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>277</v>
       </c>
       <c r="G17">
-        <v>1983</v>
+        <v>1964</v>
       </c>
       <c r="H17" s="1">
-        <v>30666</v>
-      </c>
-      <c r="I17" t="s">
-        <v>52</v>
+        <v>23700</v>
       </c>
       <c r="J17" t="s">
-        <v>53</v>
+        <v>220</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
@@ -2262,31 +2242,28 @@
         <v>201</v>
       </c>
       <c r="B18">
-        <v>13636</v>
+        <v>13147</v>
       </c>
       <c r="C18" t="s">
-        <v>72</v>
+        <v>273</v>
       </c>
       <c r="D18" t="s">
-        <v>15</v>
+        <v>234</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>73</v>
+        <v>274</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>277</v>
       </c>
       <c r="G18">
-        <v>1974</v>
+        <v>1966</v>
       </c>
       <c r="H18" s="1">
-        <v>27170</v>
-      </c>
-      <c r="I18" t="s">
-        <v>74</v>
+        <v>24415</v>
       </c>
       <c r="J18" t="s">
-        <v>75</v>
+        <v>275</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
@@ -2294,31 +2271,28 @@
         <v>201</v>
       </c>
       <c r="B19">
-        <v>13637</v>
+        <v>13084</v>
       </c>
       <c r="C19" t="s">
-        <v>112</v>
+        <v>212</v>
       </c>
       <c r="D19" t="s">
-        <v>15</v>
+        <v>128</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>113</v>
+        <v>213</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>277</v>
       </c>
       <c r="G19">
-        <v>1954</v>
+        <v>1966</v>
       </c>
       <c r="H19" s="1">
-        <v>19858</v>
-      </c>
-      <c r="I19" t="s">
-        <v>114</v>
+        <v>24385</v>
       </c>
       <c r="J19" t="s">
-        <v>115</v>
+        <v>214</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
@@ -2326,31 +2300,28 @@
         <v>201</v>
       </c>
       <c r="B20">
-        <v>13645</v>
+        <v>13085</v>
       </c>
       <c r="C20" t="s">
-        <v>99</v>
+        <v>209</v>
       </c>
       <c r="D20" t="s">
-        <v>15</v>
+        <v>128</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>100</v>
+        <v>210</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>277</v>
       </c>
       <c r="G20">
-        <v>1961</v>
+        <v>1968</v>
       </c>
       <c r="H20" s="1">
-        <v>22580</v>
-      </c>
-      <c r="I20" t="s">
-        <v>101</v>
+        <v>25161</v>
       </c>
       <c r="J20" t="s">
-        <v>102</v>
+        <v>211</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
@@ -2358,31 +2329,31 @@
         <v>201</v>
       </c>
       <c r="B21">
-        <v>13646</v>
+        <v>13039</v>
       </c>
       <c r="C21" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="D21" t="s">
         <v>15</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>277</v>
       </c>
       <c r="G21">
-        <v>1971</v>
+        <v>1970</v>
       </c>
       <c r="H21" s="1">
-        <v>26235</v>
+        <v>25886</v>
       </c>
       <c r="I21" t="s">
-        <v>91</v>
+        <v>17</v>
       </c>
       <c r="J21" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
@@ -2390,31 +2361,28 @@
         <v>201</v>
       </c>
       <c r="B22">
-        <v>15218</v>
+        <v>13086</v>
       </c>
       <c r="C22" t="s">
-        <v>61</v>
+        <v>206</v>
       </c>
       <c r="D22" t="s">
-        <v>15</v>
+        <v>128</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>62</v>
+        <v>207</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>277</v>
       </c>
       <c r="G22">
-        <v>1979</v>
+        <v>1970</v>
       </c>
       <c r="H22" s="1">
-        <v>29202</v>
-      </c>
-      <c r="I22" t="s">
-        <v>63</v>
+        <v>25885</v>
       </c>
       <c r="J22" t="s">
-        <v>64</v>
+        <v>208</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
@@ -2422,16 +2390,16 @@
         <v>201</v>
       </c>
       <c r="B23">
-        <v>15241</v>
+        <v>13646</v>
       </c>
       <c r="C23" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="D23" t="s">
         <v>15</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>277</v>
@@ -2440,13 +2408,13 @@
         <v>1971</v>
       </c>
       <c r="H23" s="1">
-        <v>26138</v>
+        <v>26235</v>
       </c>
       <c r="I23" t="s">
-        <v>17</v>
+        <v>91</v>
       </c>
       <c r="J23" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
@@ -2454,31 +2422,31 @@
         <v>201</v>
       </c>
       <c r="B24">
-        <v>15321</v>
+        <v>15241</v>
       </c>
       <c r="C24" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="D24" t="s">
         <v>15</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>277</v>
       </c>
       <c r="G24">
-        <v>1962</v>
+        <v>1971</v>
       </c>
       <c r="H24" s="1">
-        <v>22990</v>
+        <v>26138</v>
       </c>
       <c r="I24" t="s">
         <v>17</v>
       </c>
       <c r="J24" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
@@ -2486,31 +2454,31 @@
         <v>201</v>
       </c>
       <c r="B25">
-        <v>15381</v>
+        <v>15398</v>
       </c>
       <c r="C25" t="s">
-        <v>116</v>
+        <v>85</v>
       </c>
       <c r="D25" t="s">
         <v>15</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>117</v>
+        <v>86</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>277</v>
       </c>
       <c r="G25">
-        <v>1952</v>
+        <v>1971</v>
       </c>
       <c r="H25" s="1">
-        <v>19243</v>
+        <v>25966</v>
       </c>
       <c r="I25" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="J25" t="s">
-        <v>118</v>
+        <v>88</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
@@ -2518,31 +2486,31 @@
         <v>201</v>
       </c>
       <c r="B26">
-        <v>15395</v>
+        <v>13055</v>
       </c>
       <c r="C26" t="s">
-        <v>106</v>
+        <v>79</v>
       </c>
       <c r="D26" t="s">
         <v>15</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>107</v>
+        <v>80</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>277</v>
       </c>
       <c r="G26">
-        <v>1958</v>
+        <v>1972</v>
       </c>
       <c r="H26" s="1">
-        <v>21522</v>
+        <v>26619</v>
       </c>
       <c r="I26" t="s">
         <v>17</v>
       </c>
       <c r="J26" t="s">
-        <v>108</v>
+        <v>81</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
@@ -2550,31 +2518,28 @@
         <v>201</v>
       </c>
       <c r="B27">
-        <v>15398</v>
+        <v>17518</v>
       </c>
       <c r="C27" t="s">
-        <v>85</v>
+        <v>270</v>
       </c>
       <c r="D27" t="s">
-        <v>15</v>
+        <v>234</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>86</v>
+        <v>271</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>277</v>
       </c>
       <c r="G27">
-        <v>1971</v>
+        <v>1972</v>
       </c>
       <c r="H27" s="1">
-        <v>25966</v>
-      </c>
-      <c r="I27" t="s">
-        <v>87</v>
+        <v>26618</v>
       </c>
       <c r="J27" t="s">
-        <v>88</v>
+        <v>272</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
@@ -2582,31 +2547,28 @@
         <v>201</v>
       </c>
       <c r="B28">
-        <v>17716</v>
+        <v>13087</v>
       </c>
       <c r="C28" t="s">
-        <v>37</v>
+        <v>203</v>
       </c>
       <c r="D28" t="s">
-        <v>15</v>
+        <v>128</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>38</v>
+        <v>204</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G28">
-        <v>2003</v>
+        <v>1972</v>
       </c>
       <c r="H28" s="1">
-        <v>37911</v>
-      </c>
-      <c r="I28" t="s">
-        <v>17</v>
+        <v>26619</v>
       </c>
       <c r="J28" t="s">
-        <v>39</v>
+        <v>205</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
@@ -2614,31 +2576,31 @@
         <v>201</v>
       </c>
       <c r="B29">
-        <v>31037</v>
+        <v>13512</v>
       </c>
       <c r="C29" t="s">
-        <v>34</v>
+        <v>76</v>
       </c>
       <c r="D29" t="s">
         <v>15</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>35</v>
+        <v>77</v>
       </c>
       <c r="F29" s="2" t="s">
         <v>277</v>
       </c>
       <c r="G29">
-        <v>2005</v>
+        <v>1974</v>
       </c>
       <c r="H29" s="1">
-        <v>38644</v>
+        <v>27229</v>
       </c>
       <c r="I29" t="s">
-        <v>17</v>
+        <v>78</v>
       </c>
       <c r="J29" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
@@ -2646,31 +2608,31 @@
         <v>201</v>
       </c>
       <c r="B30">
-        <v>31038</v>
+        <v>13636</v>
       </c>
       <c r="C30" t="s">
-        <v>31</v>
+        <v>72</v>
       </c>
       <c r="D30" t="s">
         <v>15</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>32</v>
+        <v>73</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>277</v>
       </c>
       <c r="G30">
-        <v>2005</v>
+        <v>1974</v>
       </c>
       <c r="H30" s="1">
-        <v>38645</v>
+        <v>27170</v>
       </c>
       <c r="I30" t="s">
-        <v>17</v>
+        <v>74</v>
       </c>
       <c r="J30" t="s">
-        <v>33</v>
+        <v>75</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
@@ -2678,31 +2640,28 @@
         <v>201</v>
       </c>
       <c r="B31">
-        <v>48975</v>
+        <v>13088</v>
       </c>
       <c r="C31" t="s">
-        <v>27</v>
+        <v>200</v>
       </c>
       <c r="D31" t="s">
-        <v>15</v>
+        <v>128</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>28</v>
+        <v>201</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>277</v>
       </c>
       <c r="G31">
-        <v>2011</v>
+        <v>1974</v>
       </c>
       <c r="H31" s="1">
-        <v>40873</v>
-      </c>
-      <c r="I31" t="s">
-        <v>29</v>
+        <v>27352</v>
       </c>
       <c r="J31" t="s">
-        <v>30</v>
+        <v>202</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
@@ -2710,31 +2669,31 @@
         <v>201</v>
       </c>
       <c r="B32">
-        <v>49282</v>
+        <v>13514</v>
       </c>
       <c r="C32" t="s">
-        <v>23</v>
+        <v>68</v>
       </c>
       <c r="D32" t="s">
         <v>15</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>24</v>
+        <v>69</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>277</v>
       </c>
       <c r="G32">
-        <v>2014</v>
+        <v>1976</v>
       </c>
       <c r="H32" s="1">
-        <v>41985</v>
+        <v>28111</v>
       </c>
       <c r="I32" t="s">
-        <v>25</v>
+        <v>70</v>
       </c>
       <c r="J32" t="s">
-        <v>26</v>
+        <v>71</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
@@ -2742,31 +2701,28 @@
         <v>201</v>
       </c>
       <c r="B33">
-        <v>49523</v>
+        <v>13089</v>
       </c>
       <c r="C33" t="s">
-        <v>19</v>
+        <v>194</v>
       </c>
       <c r="D33" t="s">
-        <v>15</v>
+        <v>128</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>20</v>
+        <v>195</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>277</v>
       </c>
       <c r="G33">
-        <v>2019</v>
+        <v>1976</v>
       </c>
       <c r="H33" s="1">
-        <v>43659</v>
-      </c>
-      <c r="I33" t="s">
-        <v>21</v>
+        <v>28086</v>
       </c>
       <c r="J33" t="s">
-        <v>22</v>
+        <v>196</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
@@ -2774,31 +2730,28 @@
         <v>201</v>
       </c>
       <c r="B34">
-        <v>49557</v>
+        <v>13092</v>
       </c>
       <c r="C34" t="s">
-        <v>14</v>
+        <v>191</v>
       </c>
       <c r="D34" t="s">
-        <v>15</v>
+        <v>128</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>16</v>
+        <v>192</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G34">
-        <v>2019</v>
+        <v>1976</v>
       </c>
       <c r="H34" s="1">
-        <v>43794</v>
-      </c>
-      <c r="I34" t="s">
-        <v>17</v>
+        <v>28086</v>
       </c>
       <c r="J34" t="s">
-        <v>18</v>
+        <v>193</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
@@ -2806,28 +2759,28 @@
         <v>201</v>
       </c>
       <c r="B35">
-        <v>13147</v>
+        <v>13097</v>
       </c>
       <c r="C35" t="s">
-        <v>273</v>
+        <v>197</v>
       </c>
       <c r="D35" t="s">
-        <v>234</v>
+        <v>128</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>274</v>
+        <v>198</v>
       </c>
       <c r="F35" s="2" t="s">
         <v>277</v>
       </c>
       <c r="G35">
-        <v>1966</v>
+        <v>1976</v>
       </c>
       <c r="H35" s="1">
-        <v>24415</v>
+        <v>28090</v>
       </c>
       <c r="J35" t="s">
-        <v>275</v>
+        <v>199</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
@@ -2835,28 +2788,28 @@
         <v>201</v>
       </c>
       <c r="B36">
-        <v>13150</v>
+        <v>13132</v>
       </c>
       <c r="C36" t="s">
-        <v>237</v>
+        <v>185</v>
       </c>
       <c r="D36" t="s">
-        <v>234</v>
+        <v>128</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>238</v>
+        <v>186</v>
       </c>
       <c r="F36" s="2" t="s">
         <v>277</v>
       </c>
       <c r="G36">
-        <v>2015</v>
+        <v>1976</v>
       </c>
       <c r="H36" s="1">
-        <v>42325</v>
+        <v>28090</v>
       </c>
       <c r="J36" t="s">
-        <v>239</v>
+        <v>187</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
@@ -2864,28 +2817,28 @@
         <v>201</v>
       </c>
       <c r="B37">
-        <v>13161</v>
+        <v>13133</v>
       </c>
       <c r="C37" t="s">
-        <v>264</v>
+        <v>188</v>
       </c>
       <c r="D37" t="s">
-        <v>234</v>
+        <v>128</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>265</v>
+        <v>189</v>
       </c>
       <c r="F37" s="2" t="s">
         <v>277</v>
       </c>
       <c r="G37">
-        <v>1978</v>
+        <v>1976</v>
       </c>
       <c r="H37" s="1">
-        <v>28821</v>
+        <v>28090</v>
       </c>
       <c r="J37" t="s">
-        <v>266</v>
+        <v>190</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
@@ -2893,28 +2846,31 @@
         <v>201</v>
       </c>
       <c r="B38">
-        <v>13175</v>
+        <v>13517</v>
       </c>
       <c r="C38" t="s">
-        <v>261</v>
+        <v>65</v>
       </c>
       <c r="D38" t="s">
-        <v>234</v>
+        <v>15</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>262</v>
+        <v>66</v>
       </c>
       <c r="F38" s="2" t="s">
         <v>277</v>
       </c>
       <c r="G38">
-        <v>1995</v>
+        <v>1978</v>
       </c>
       <c r="H38" s="1">
-        <v>35019</v>
+        <v>28846</v>
+      </c>
+      <c r="I38" t="s">
+        <v>17</v>
       </c>
       <c r="J38" t="s">
-        <v>263</v>
+        <v>67</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
@@ -2922,16 +2878,16 @@
         <v>201</v>
       </c>
       <c r="B39">
-        <v>13176</v>
+        <v>13161</v>
       </c>
       <c r="C39" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="D39" t="s">
         <v>234</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="F39" s="2" t="s">
         <v>277</v>
@@ -2940,10 +2896,10 @@
         <v>1978</v>
       </c>
       <c r="H39" s="1">
-        <v>28822</v>
+        <v>28821</v>
       </c>
       <c r="J39" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
@@ -2951,28 +2907,28 @@
         <v>201</v>
       </c>
       <c r="B40">
-        <v>13177</v>
+        <v>13176</v>
       </c>
       <c r="C40" t="s">
-        <v>255</v>
+        <v>267</v>
       </c>
       <c r="D40" t="s">
         <v>234</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>256</v>
+        <v>268</v>
       </c>
       <c r="F40" s="2" t="s">
         <v>277</v>
       </c>
       <c r="G40">
-        <v>1997</v>
+        <v>1978</v>
       </c>
       <c r="H40" s="1">
-        <v>35745</v>
+        <v>28822</v>
       </c>
       <c r="J40" t="s">
-        <v>257</v>
+        <v>269</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
@@ -2980,28 +2936,28 @@
         <v>201</v>
       </c>
       <c r="B41">
-        <v>13178</v>
+        <v>13134</v>
       </c>
       <c r="C41" t="s">
-        <v>258</v>
+        <v>173</v>
       </c>
       <c r="D41" t="s">
-        <v>234</v>
+        <v>128</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>259</v>
+        <v>174</v>
       </c>
       <c r="F41" s="2" t="s">
         <v>277</v>
       </c>
       <c r="G41">
-        <v>1997</v>
+        <v>1978</v>
       </c>
       <c r="H41" s="1">
-        <v>35746</v>
+        <v>28821</v>
       </c>
       <c r="J41" t="s">
-        <v>260</v>
+        <v>175</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
@@ -3009,28 +2965,28 @@
         <v>201</v>
       </c>
       <c r="B42">
-        <v>13179</v>
+        <v>13135</v>
       </c>
       <c r="C42" t="s">
-        <v>252</v>
+        <v>176</v>
       </c>
       <c r="D42" t="s">
-        <v>234</v>
+        <v>128</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>253</v>
+        <v>177</v>
       </c>
       <c r="F42" s="2" t="s">
         <v>277</v>
       </c>
       <c r="G42">
-        <v>2001</v>
+        <v>1978</v>
       </c>
       <c r="H42" s="1">
-        <v>37197</v>
+        <v>28821</v>
       </c>
       <c r="J42" t="s">
-        <v>254</v>
+        <v>178</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
@@ -3038,28 +2994,28 @@
         <v>201</v>
       </c>
       <c r="B43">
-        <v>17518</v>
+        <v>13136</v>
       </c>
       <c r="C43" t="s">
-        <v>270</v>
+        <v>179</v>
       </c>
       <c r="D43" t="s">
-        <v>234</v>
+        <v>128</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>271</v>
+        <v>180</v>
       </c>
       <c r="F43" s="2" t="s">
         <v>277</v>
       </c>
       <c r="G43">
-        <v>1972</v>
+        <v>1978</v>
       </c>
       <c r="H43" s="1">
-        <v>26618</v>
+        <v>28821</v>
       </c>
       <c r="J43" t="s">
-        <v>272</v>
+        <v>181</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.2">
@@ -3067,28 +3023,28 @@
         <v>201</v>
       </c>
       <c r="B44">
-        <v>17718</v>
+        <v>13137</v>
       </c>
       <c r="C44" t="s">
-        <v>243</v>
+        <v>182</v>
       </c>
       <c r="D44" t="s">
-        <v>234</v>
+        <v>128</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>244</v>
+        <v>183</v>
       </c>
       <c r="F44" s="2" t="s">
         <v>277</v>
       </c>
       <c r="G44">
-        <v>2003</v>
+        <v>1978</v>
       </c>
       <c r="H44" s="1">
-        <v>37911</v>
+        <v>28822</v>
       </c>
       <c r="J44" t="s">
-        <v>245</v>
+        <v>184</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.2">
@@ -3096,28 +3052,31 @@
         <v>201</v>
       </c>
       <c r="B45">
-        <v>17720</v>
+        <v>13516</v>
       </c>
       <c r="C45" t="s">
-        <v>246</v>
+        <v>58</v>
       </c>
       <c r="D45" t="s">
-        <v>234</v>
+        <v>15</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>247</v>
+        <v>59</v>
       </c>
       <c r="F45" s="2" t="s">
         <v>277</v>
       </c>
       <c r="G45">
-        <v>2003</v>
+        <v>1979</v>
       </c>
       <c r="H45" s="1">
-        <v>37910</v>
+        <v>29210</v>
+      </c>
+      <c r="I45" t="s">
+        <v>17</v>
       </c>
       <c r="J45" t="s">
-        <v>248</v>
+        <v>60</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.2">
@@ -3125,28 +3084,31 @@
         <v>201</v>
       </c>
       <c r="B46">
-        <v>17721</v>
+        <v>15218</v>
       </c>
       <c r="C46" t="s">
-        <v>249</v>
+        <v>61</v>
       </c>
       <c r="D46" t="s">
-        <v>234</v>
+        <v>15</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>250</v>
+        <v>62</v>
       </c>
       <c r="F46" s="2" t="s">
         <v>277</v>
       </c>
       <c r="G46">
-        <v>2003</v>
+        <v>1979</v>
       </c>
       <c r="H46" s="1">
-        <v>37909</v>
+        <v>29202</v>
+      </c>
+      <c r="I46" t="s">
+        <v>63</v>
       </c>
       <c r="J46" t="s">
-        <v>251</v>
+        <v>64</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
@@ -3154,28 +3116,28 @@
         <v>201</v>
       </c>
       <c r="B47">
-        <v>31058</v>
+        <v>13138</v>
       </c>
       <c r="C47" t="s">
-        <v>240</v>
+        <v>164</v>
       </c>
       <c r="D47" t="s">
-        <v>234</v>
+        <v>128</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>241</v>
+        <v>165</v>
       </c>
       <c r="F47" s="2" t="s">
         <v>277</v>
       </c>
       <c r="G47">
-        <v>2005</v>
+        <v>1980</v>
       </c>
       <c r="H47" s="1">
-        <v>38644</v>
+        <v>29521</v>
       </c>
       <c r="J47" t="s">
-        <v>242</v>
+        <v>166</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.2">
@@ -3183,28 +3145,28 @@
         <v>201</v>
       </c>
       <c r="B48">
-        <v>49457</v>
+        <v>13139</v>
       </c>
       <c r="C48" t="s">
-        <v>233</v>
+        <v>167</v>
       </c>
       <c r="D48" t="s">
-        <v>234</v>
+        <v>128</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>235</v>
+        <v>168</v>
       </c>
       <c r="F48" s="2" t="s">
         <v>277</v>
       </c>
       <c r="G48">
-        <v>2017</v>
+        <v>1980</v>
       </c>
       <c r="H48" s="1">
-        <v>43052</v>
+        <v>29521</v>
       </c>
       <c r="J48" t="s">
-        <v>236</v>
+        <v>169</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.2">
@@ -3212,28 +3174,28 @@
         <v>201</v>
       </c>
       <c r="B49">
-        <v>13062</v>
+        <v>13140</v>
       </c>
       <c r="C49" t="s">
-        <v>230</v>
+        <v>170</v>
       </c>
       <c r="D49" t="s">
         <v>128</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>231</v>
+        <v>171</v>
       </c>
       <c r="F49" s="2" t="s">
         <v>277</v>
       </c>
       <c r="G49">
-        <v>1956</v>
+        <v>1980</v>
       </c>
       <c r="H49" s="1">
-        <v>20794</v>
+        <v>29521</v>
       </c>
       <c r="J49" t="s">
-        <v>232</v>
+        <v>172</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.2">
@@ -3241,28 +3203,31 @@
         <v>201</v>
       </c>
       <c r="B50">
-        <v>13063</v>
+        <v>13518</v>
       </c>
       <c r="C50" t="s">
-        <v>224</v>
+        <v>54</v>
       </c>
       <c r="D50" t="s">
-        <v>128</v>
+        <v>15</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>225</v>
+        <v>55</v>
       </c>
       <c r="F50" s="2" t="s">
         <v>277</v>
       </c>
       <c r="G50">
-        <v>1960</v>
+        <v>1981</v>
       </c>
       <c r="H50" s="1">
-        <v>22264</v>
+        <v>29925</v>
+      </c>
+      <c r="I50" t="s">
+        <v>56</v>
       </c>
       <c r="J50" t="s">
-        <v>226</v>
+        <v>57</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.2">
@@ -3270,28 +3235,31 @@
         <v>201</v>
       </c>
       <c r="B51">
-        <v>13065</v>
+        <v>13523</v>
       </c>
       <c r="C51" t="s">
-        <v>227</v>
+        <v>50</v>
       </c>
       <c r="D51" t="s">
-        <v>128</v>
+        <v>15</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>228</v>
+        <v>51</v>
       </c>
       <c r="F51" s="2" t="s">
         <v>277</v>
       </c>
       <c r="G51">
-        <v>1960</v>
+        <v>1983</v>
       </c>
       <c r="H51" s="1">
-        <v>22264</v>
+        <v>30666</v>
+      </c>
+      <c r="I51" t="s">
+        <v>52</v>
       </c>
       <c r="J51" t="s">
-        <v>229</v>
+        <v>53</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.2">
@@ -3299,28 +3267,28 @@
         <v>201</v>
       </c>
       <c r="B52">
-        <v>13067</v>
+        <v>13146</v>
       </c>
       <c r="C52" t="s">
-        <v>221</v>
+        <v>161</v>
       </c>
       <c r="D52" t="s">
         <v>128</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>222</v>
+        <v>162</v>
       </c>
       <c r="F52" s="2" t="s">
         <v>277</v>
       </c>
       <c r="G52">
-        <v>1962</v>
+        <v>1985</v>
       </c>
       <c r="H52" s="1">
-        <v>22991</v>
+        <v>31352</v>
       </c>
       <c r="J52" t="s">
-        <v>223</v>
+        <v>163</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.2">
@@ -3328,28 +3296,31 @@
         <v>201</v>
       </c>
       <c r="B53">
-        <v>13068</v>
+        <v>13059</v>
       </c>
       <c r="C53" t="s">
-        <v>215</v>
+        <v>47</v>
       </c>
       <c r="D53" t="s">
-        <v>128</v>
+        <v>15</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>216</v>
+        <v>48</v>
       </c>
       <c r="F53" s="2" t="s">
         <v>277</v>
       </c>
       <c r="G53">
-        <v>1964</v>
+        <v>1989</v>
       </c>
       <c r="H53" s="1">
-        <v>23700</v>
+        <v>32822</v>
+      </c>
+      <c r="I53" t="s">
+        <v>17</v>
       </c>
       <c r="J53" t="s">
-        <v>217</v>
+        <v>49</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.2">
@@ -3357,28 +3328,28 @@
         <v>201</v>
       </c>
       <c r="B54">
-        <v>13083</v>
+        <v>13141</v>
       </c>
       <c r="C54" t="s">
-        <v>218</v>
+        <v>158</v>
       </c>
       <c r="D54" t="s">
         <v>128</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>219</v>
+        <v>159</v>
       </c>
       <c r="F54" s="2" t="s">
         <v>277</v>
       </c>
       <c r="G54">
-        <v>1964</v>
+        <v>1989</v>
       </c>
       <c r="H54" s="1">
-        <v>23700</v>
+        <v>32827</v>
       </c>
       <c r="J54" t="s">
-        <v>220</v>
+        <v>160</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.2">
@@ -3386,28 +3357,28 @@
         <v>201</v>
       </c>
       <c r="B55">
-        <v>13084</v>
+        <v>13142</v>
       </c>
       <c r="C55" t="s">
-        <v>212</v>
+        <v>155</v>
       </c>
       <c r="D55" t="s">
         <v>128</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>213</v>
+        <v>156</v>
       </c>
       <c r="F55" s="2" t="s">
         <v>277</v>
       </c>
       <c r="G55">
-        <v>1966</v>
+        <v>1993</v>
       </c>
       <c r="H55" s="1">
-        <v>24385</v>
+        <v>34286</v>
       </c>
       <c r="J55" t="s">
-        <v>214</v>
+        <v>157</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.2">
@@ -3415,28 +3386,28 @@
         <v>201</v>
       </c>
       <c r="B56">
-        <v>13085</v>
+        <v>13175</v>
       </c>
       <c r="C56" t="s">
-        <v>209</v>
+        <v>261</v>
       </c>
       <c r="D56" t="s">
-        <v>128</v>
+        <v>234</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>210</v>
+        <v>262</v>
       </c>
       <c r="F56" s="2" t="s">
         <v>277</v>
       </c>
       <c r="G56">
-        <v>1968</v>
+        <v>1995</v>
       </c>
       <c r="H56" s="1">
-        <v>25161</v>
+        <v>35019</v>
       </c>
       <c r="J56" t="s">
-        <v>211</v>
+        <v>263</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.2">
@@ -3444,28 +3415,31 @@
         <v>201</v>
       </c>
       <c r="B57">
-        <v>13086</v>
+        <v>13522</v>
       </c>
       <c r="C57" t="s">
-        <v>206</v>
+        <v>43</v>
       </c>
       <c r="D57" t="s">
-        <v>128</v>
+        <v>15</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>207</v>
+        <v>44</v>
       </c>
       <c r="F57" s="2" t="s">
         <v>277</v>
       </c>
       <c r="G57">
-        <v>1970</v>
+        <v>1997</v>
       </c>
       <c r="H57" s="1">
-        <v>25885</v>
+        <v>35531</v>
+      </c>
+      <c r="I57" t="s">
+        <v>45</v>
       </c>
       <c r="J57" t="s">
-        <v>208</v>
+        <v>46</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.2">
@@ -3473,28 +3447,28 @@
         <v>201</v>
       </c>
       <c r="B58">
-        <v>13087</v>
+        <v>13177</v>
       </c>
       <c r="C58" t="s">
-        <v>203</v>
+        <v>255</v>
       </c>
       <c r="D58" t="s">
-        <v>128</v>
+        <v>234</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>204</v>
+        <v>256</v>
       </c>
       <c r="F58" s="2" t="s">
         <v>277</v>
       </c>
       <c r="G58">
-        <v>1972</v>
+        <v>1997</v>
       </c>
       <c r="H58" s="1">
-        <v>26619</v>
+        <v>35745</v>
       </c>
       <c r="J58" t="s">
-        <v>205</v>
+        <v>257</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.2">
@@ -3502,28 +3476,28 @@
         <v>201</v>
       </c>
       <c r="B59">
-        <v>13088</v>
+        <v>13178</v>
       </c>
       <c r="C59" t="s">
-        <v>200</v>
+        <v>258</v>
       </c>
       <c r="D59" t="s">
-        <v>128</v>
+        <v>234</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>201</v>
+        <v>259</v>
       </c>
       <c r="F59" s="2" t="s">
         <v>277</v>
       </c>
       <c r="G59">
-        <v>1974</v>
+        <v>1997</v>
       </c>
       <c r="H59" s="1">
-        <v>27352</v>
+        <v>35746</v>
       </c>
       <c r="J59" t="s">
-        <v>202</v>
+        <v>260</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.2">
@@ -3531,28 +3505,28 @@
         <v>201</v>
       </c>
       <c r="B60">
-        <v>13089</v>
+        <v>13144</v>
       </c>
       <c r="C60" t="s">
-        <v>194</v>
+        <v>152</v>
       </c>
       <c r="D60" t="s">
         <v>128</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>195</v>
+        <v>153</v>
       </c>
       <c r="F60" s="2" t="s">
         <v>277</v>
       </c>
       <c r="G60">
-        <v>1976</v>
+        <v>1997</v>
       </c>
       <c r="H60" s="1">
-        <v>28086</v>
+        <v>35745</v>
       </c>
       <c r="J60" t="s">
-        <v>196</v>
+        <v>154</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.2">
@@ -3560,28 +3534,31 @@
         <v>201</v>
       </c>
       <c r="B61">
-        <v>13092</v>
+        <v>13520</v>
       </c>
       <c r="C61" t="s">
-        <v>191</v>
+        <v>40</v>
       </c>
       <c r="D61" t="s">
-        <v>128</v>
+        <v>15</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>192</v>
+        <v>41</v>
       </c>
       <c r="F61" s="2" t="s">
         <v>277</v>
       </c>
       <c r="G61">
-        <v>1976</v>
+        <v>2001</v>
       </c>
       <c r="H61" s="1">
-        <v>28086</v>
+        <v>37197</v>
+      </c>
+      <c r="I61" t="s">
+        <v>17</v>
       </c>
       <c r="J61" t="s">
-        <v>193</v>
+        <v>42</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.2">
@@ -3589,28 +3566,28 @@
         <v>201</v>
       </c>
       <c r="B62">
-        <v>13097</v>
+        <v>13179</v>
       </c>
       <c r="C62" t="s">
-        <v>197</v>
+        <v>252</v>
       </c>
       <c r="D62" t="s">
-        <v>128</v>
+        <v>234</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>198</v>
+        <v>253</v>
       </c>
       <c r="F62" s="2" t="s">
         <v>277</v>
       </c>
       <c r="G62">
-        <v>1976</v>
+        <v>2001</v>
       </c>
       <c r="H62" s="1">
-        <v>28090</v>
+        <v>37197</v>
       </c>
       <c r="J62" t="s">
-        <v>199</v>
+        <v>254</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.2">
@@ -3618,28 +3595,31 @@
         <v>201</v>
       </c>
       <c r="B63">
-        <v>13132</v>
+        <v>17716</v>
       </c>
       <c r="C63" t="s">
-        <v>185</v>
+        <v>37</v>
       </c>
       <c r="D63" t="s">
-        <v>128</v>
+        <v>15</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>186</v>
+        <v>38</v>
       </c>
       <c r="F63" s="2" t="s">
         <v>277</v>
       </c>
       <c r="G63">
-        <v>1976</v>
+        <v>2003</v>
       </c>
       <c r="H63" s="1">
-        <v>28090</v>
+        <v>37911</v>
+      </c>
+      <c r="I63" t="s">
+        <v>17</v>
       </c>
       <c r="J63" t="s">
-        <v>187</v>
+        <v>39</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.2">
@@ -3647,28 +3627,28 @@
         <v>201</v>
       </c>
       <c r="B64">
-        <v>13133</v>
+        <v>17718</v>
       </c>
       <c r="C64" t="s">
-        <v>188</v>
+        <v>243</v>
       </c>
       <c r="D64" t="s">
-        <v>128</v>
+        <v>234</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>189</v>
+        <v>244</v>
       </c>
       <c r="F64" s="2" t="s">
         <v>277</v>
       </c>
       <c r="G64">
-        <v>1976</v>
+        <v>2003</v>
       </c>
       <c r="H64" s="1">
-        <v>28090</v>
+        <v>37911</v>
       </c>
       <c r="J64" t="s">
-        <v>190</v>
+        <v>245</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.2">
@@ -3676,28 +3656,28 @@
         <v>201</v>
       </c>
       <c r="B65">
-        <v>13134</v>
+        <v>17720</v>
       </c>
       <c r="C65" t="s">
-        <v>173</v>
+        <v>246</v>
       </c>
       <c r="D65" t="s">
-        <v>128</v>
+        <v>234</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>174</v>
+        <v>247</v>
       </c>
       <c r="F65" s="2" t="s">
         <v>277</v>
       </c>
       <c r="G65">
-        <v>1978</v>
+        <v>2003</v>
       </c>
       <c r="H65" s="1">
-        <v>28821</v>
+        <v>37910</v>
       </c>
       <c r="J65" t="s">
-        <v>175</v>
+        <v>248</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.2">
@@ -3705,28 +3685,28 @@
         <v>201</v>
       </c>
       <c r="B66">
-        <v>13135</v>
+        <v>17721</v>
       </c>
       <c r="C66" t="s">
-        <v>176</v>
+        <v>249</v>
       </c>
       <c r="D66" t="s">
-        <v>128</v>
+        <v>234</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>177</v>
+        <v>250</v>
       </c>
       <c r="F66" s="2" t="s">
         <v>277</v>
       </c>
       <c r="G66">
-        <v>1978</v>
+        <v>2003</v>
       </c>
       <c r="H66" s="1">
-        <v>28821</v>
+        <v>37909</v>
       </c>
       <c r="J66" t="s">
-        <v>178</v>
+        <v>251</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.2">
@@ -3734,28 +3714,28 @@
         <v>201</v>
       </c>
       <c r="B67">
-        <v>13136</v>
+        <v>17717</v>
       </c>
       <c r="C67" t="s">
-        <v>179</v>
+        <v>149</v>
       </c>
       <c r="D67" t="s">
         <v>128</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>180</v>
+        <v>150</v>
       </c>
       <c r="F67" s="2" t="s">
         <v>277</v>
       </c>
       <c r="G67">
-        <v>1978</v>
+        <v>2003</v>
       </c>
       <c r="H67" s="1">
-        <v>28821</v>
+        <v>37909</v>
       </c>
       <c r="J67" t="s">
-        <v>181</v>
+        <v>151</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.2">
@@ -3763,28 +3743,31 @@
         <v>201</v>
       </c>
       <c r="B68">
-        <v>13137</v>
+        <v>31037</v>
       </c>
       <c r="C68" t="s">
-        <v>182</v>
+        <v>34</v>
       </c>
       <c r="D68" t="s">
-        <v>128</v>
+        <v>15</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>183</v>
+        <v>35</v>
       </c>
       <c r="F68" s="2" t="s">
         <v>277</v>
       </c>
       <c r="G68">
-        <v>1978</v>
+        <v>2005</v>
       </c>
       <c r="H68" s="1">
-        <v>28822</v>
+        <v>38644</v>
+      </c>
+      <c r="I68" t="s">
+        <v>17</v>
       </c>
       <c r="J68" t="s">
-        <v>184</v>
+        <v>36</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.2">
@@ -3792,28 +3775,31 @@
         <v>201</v>
       </c>
       <c r="B69">
-        <v>13138</v>
+        <v>31038</v>
       </c>
       <c r="C69" t="s">
-        <v>164</v>
+        <v>31</v>
       </c>
       <c r="D69" t="s">
-        <v>128</v>
+        <v>15</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>165</v>
+        <v>32</v>
       </c>
       <c r="F69" s="2" t="s">
         <v>277</v>
       </c>
       <c r="G69">
-        <v>1980</v>
+        <v>2005</v>
       </c>
       <c r="H69" s="1">
-        <v>29521</v>
+        <v>38645</v>
+      </c>
+      <c r="I69" t="s">
+        <v>17</v>
       </c>
       <c r="J69" t="s">
-        <v>166</v>
+        <v>33</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.2">
@@ -3821,28 +3807,28 @@
         <v>201</v>
       </c>
       <c r="B70">
-        <v>13139</v>
+        <v>31058</v>
       </c>
       <c r="C70" t="s">
-        <v>167</v>
+        <v>240</v>
       </c>
       <c r="D70" t="s">
-        <v>128</v>
+        <v>234</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>168</v>
+        <v>241</v>
       </c>
       <c r="F70" s="2" t="s">
         <v>277</v>
       </c>
       <c r="G70">
-        <v>1980</v>
+        <v>2005</v>
       </c>
       <c r="H70" s="1">
-        <v>29521</v>
+        <v>38644</v>
       </c>
       <c r="J70" t="s">
-        <v>169</v>
+        <v>242</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.2">
@@ -3850,28 +3836,31 @@
         <v>201</v>
       </c>
       <c r="B71">
-        <v>13140</v>
+        <v>48975</v>
       </c>
       <c r="C71" t="s">
-        <v>170</v>
+        <v>27</v>
       </c>
       <c r="D71" t="s">
-        <v>128</v>
+        <v>15</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>171</v>
+        <v>28</v>
       </c>
       <c r="F71" s="2" t="s">
         <v>277</v>
       </c>
       <c r="G71">
-        <v>1980</v>
+        <v>2011</v>
       </c>
       <c r="H71" s="1">
-        <v>29521</v>
+        <v>40873</v>
+      </c>
+      <c r="I71" t="s">
+        <v>29</v>
       </c>
       <c r="J71" t="s">
-        <v>172</v>
+        <v>30</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.2">
@@ -3879,28 +3868,28 @@
         <v>201</v>
       </c>
       <c r="B72">
-        <v>13141</v>
+        <v>48857</v>
       </c>
       <c r="C72" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="D72" t="s">
         <v>128</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="F72" s="2" t="s">
         <v>277</v>
       </c>
       <c r="G72">
-        <v>1989</v>
+        <v>2011</v>
       </c>
       <c r="H72" s="1">
-        <v>32827</v>
+        <v>40857</v>
       </c>
       <c r="J72" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.2">
@@ -3908,28 +3897,31 @@
         <v>201</v>
       </c>
       <c r="B73">
-        <v>13142</v>
+        <v>49282</v>
       </c>
       <c r="C73" t="s">
-        <v>155</v>
+        <v>23</v>
       </c>
       <c r="D73" t="s">
-        <v>128</v>
+        <v>15</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>156</v>
+        <v>24</v>
       </c>
       <c r="F73" s="2" t="s">
         <v>277</v>
       </c>
       <c r="G73">
-        <v>1993</v>
+        <v>2014</v>
       </c>
       <c r="H73" s="1">
-        <v>34286</v>
+        <v>41985</v>
+      </c>
+      <c r="I73" t="s">
+        <v>25</v>
       </c>
       <c r="J73" t="s">
-        <v>157</v>
+        <v>26</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.2">
@@ -3937,28 +3929,28 @@
         <v>201</v>
       </c>
       <c r="B74">
-        <v>13144</v>
+        <v>13150</v>
       </c>
       <c r="C74" t="s">
-        <v>152</v>
+        <v>237</v>
       </c>
       <c r="D74" t="s">
-        <v>128</v>
+        <v>234</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>153</v>
+        <v>238</v>
       </c>
       <c r="F74" s="2" t="s">
         <v>277</v>
       </c>
       <c r="G74">
-        <v>1997</v>
+        <v>2015</v>
       </c>
       <c r="H74" s="1">
-        <v>35745</v>
+        <v>42325</v>
       </c>
       <c r="J74" t="s">
-        <v>154</v>
+        <v>239</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.2">
@@ -3966,28 +3958,28 @@
         <v>201</v>
       </c>
       <c r="B75">
-        <v>13146</v>
+        <v>49354</v>
       </c>
       <c r="C75" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="D75" t="s">
         <v>128</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>162</v>
+        <v>135</v>
       </c>
       <c r="F75" s="2" t="s">
         <v>277</v>
       </c>
       <c r="G75">
-        <v>1985</v>
+        <v>2015</v>
       </c>
       <c r="H75" s="1">
-        <v>31352</v>
+        <v>42321</v>
       </c>
       <c r="J75" t="s">
-        <v>163</v>
+        <v>136</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.2">
@@ -3995,28 +3987,28 @@
         <v>201</v>
       </c>
       <c r="B76">
-        <v>17717</v>
+        <v>49355</v>
       </c>
       <c r="C76" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="D76" t="s">
         <v>128</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="F76" s="2" t="s">
         <v>277</v>
       </c>
       <c r="G76">
-        <v>2003</v>
+        <v>2015</v>
       </c>
       <c r="H76" s="1">
-        <v>37909</v>
+        <v>42321</v>
       </c>
       <c r="J76" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.2">
@@ -4024,28 +4016,28 @@
         <v>201</v>
       </c>
       <c r="B77">
-        <v>48857</v>
+        <v>49357</v>
       </c>
       <c r="C77" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="D77" t="s">
         <v>128</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="F77" s="2" t="s">
         <v>277</v>
       </c>
       <c r="G77">
-        <v>2011</v>
+        <v>2015</v>
       </c>
       <c r="H77" s="1">
-        <v>40857</v>
+        <v>42325</v>
       </c>
       <c r="J77" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.2">
@@ -4053,16 +4045,16 @@
         <v>201</v>
       </c>
       <c r="B78">
-        <v>49354</v>
+        <v>49358</v>
       </c>
       <c r="C78" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="D78" t="s">
         <v>128</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
       <c r="F78" s="2" t="s">
         <v>277</v>
@@ -4071,10 +4063,10 @@
         <v>2015</v>
       </c>
       <c r="H78" s="1">
-        <v>42321</v>
+        <v>42325</v>
       </c>
       <c r="J78" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.2">
@@ -4082,28 +4074,28 @@
         <v>201</v>
       </c>
       <c r="B79">
-        <v>49355</v>
+        <v>49457</v>
       </c>
       <c r="C79" t="s">
-        <v>137</v>
+        <v>233</v>
       </c>
       <c r="D79" t="s">
-        <v>128</v>
+        <v>234</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>138</v>
+        <v>235</v>
       </c>
       <c r="F79" s="2" t="s">
         <v>277</v>
       </c>
       <c r="G79">
-        <v>2015</v>
+        <v>2017</v>
       </c>
       <c r="H79" s="1">
-        <v>42321</v>
+        <v>43052</v>
       </c>
       <c r="J79" t="s">
-        <v>139</v>
+        <v>236</v>
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.2">
@@ -4111,28 +4103,28 @@
         <v>201</v>
       </c>
       <c r="B80">
-        <v>49357</v>
+        <v>49455</v>
       </c>
       <c r="C80" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="D80" t="s">
         <v>128</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="F80" s="2" t="s">
         <v>277</v>
       </c>
       <c r="G80">
-        <v>2015</v>
+        <v>2017</v>
       </c>
       <c r="H80" s="1">
-        <v>42325</v>
+        <v>43052</v>
       </c>
       <c r="J80" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.2">
@@ -4140,28 +4132,31 @@
         <v>201</v>
       </c>
       <c r="B81">
-        <v>49358</v>
+        <v>49523</v>
       </c>
       <c r="C81" t="s">
-        <v>143</v>
+        <v>19</v>
       </c>
       <c r="D81" t="s">
-        <v>128</v>
+        <v>15</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>144</v>
+        <v>20</v>
       </c>
       <c r="F81" s="2" t="s">
         <v>277</v>
       </c>
       <c r="G81">
-        <v>2015</v>
+        <v>2019</v>
       </c>
       <c r="H81" s="1">
-        <v>42325</v>
+        <v>43659</v>
+      </c>
+      <c r="I81" t="s">
+        <v>21</v>
       </c>
       <c r="J81" t="s">
-        <v>145</v>
+        <v>22</v>
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.2">
@@ -4169,28 +4164,31 @@
         <v>201</v>
       </c>
       <c r="B82">
-        <v>49455</v>
+        <v>49557</v>
       </c>
       <c r="C82" t="s">
-        <v>131</v>
+        <v>14</v>
       </c>
       <c r="D82" t="s">
-        <v>128</v>
+        <v>15</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>132</v>
+        <v>16</v>
       </c>
       <c r="F82" s="2" t="s">
         <v>277</v>
       </c>
       <c r="G82">
-        <v>2017</v>
+        <v>2019</v>
       </c>
       <c r="H82" s="1">
-        <v>43052</v>
+        <v>43794</v>
+      </c>
+      <c r="I82" t="s">
+        <v>17</v>
       </c>
       <c r="J82" t="s">
-        <v>133</v>
+        <v>18</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.2">
@@ -4225,8 +4223,7 @@
   </sheetData>
   <autoFilter ref="A1:J83" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <sortState ref="A2:J83">
-      <sortCondition ref="D2:D83"/>
-      <sortCondition ref="B2:B83"/>
+      <sortCondition ref="G1:G83"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
spelling checks to SSI files
</commit_message>
<xml_diff>
--- a/data/legal_instrument_index.xlsx
+++ b/data/legal_instrument_index.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benjaminmartin/Documents/Academic Work (non-diss)/Intl Ideas at UNESCO (VR 2020-2023)/INIDUN/unesco_data_collection/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13B150D7-AF0F-2A4E-9999-9647F681621E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3802C906-84B4-9A4E-9B1A-596BF9E89014}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5720" yWindow="880" windowWidth="27640" windowHeight="16540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1702,8 +1702,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:J83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="A65" sqref="A65"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>